<commit_message>
update alm ev/rki ifsg für corona report
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-01-17.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-01-17.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="227">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -27,7 +27,7 @@
     <t xml:space="preserve">Vorwoche</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 1</t>
+    <t xml:space="preserve">KW 2</t>
   </si>
   <si>
     <t xml:space="preserve">Veraenderung</t>
@@ -36,79 +36,76 @@
     <t xml:space="preserve">Zahl der PCR-Tests</t>
   </si>
   <si>
-    <t xml:space="preserve">721463</t>
-  </si>
-  <si>
     <t xml:space="preserve">1062585</t>
   </si>
   <si>
-    <t xml:space="preserve">47 %</t>
+    <t xml:space="preserve">1056969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1 %</t>
   </si>
   <si>
     <t xml:space="preserve">Positive Tests</t>
   </si>
   <si>
-    <t xml:space="preserve">118645</t>
-  </si>
-  <si>
     <t xml:space="preserve">145358</t>
   </si>
   <si>
-    <t xml:space="preserve">22,5 %</t>
+    <t xml:space="preserve">113893</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-21,6 %</t>
   </si>
   <si>
     <t xml:space="preserve">Positivrate</t>
   </si>
   <si>
-    <t xml:space="preserve">16,45 %</t>
-  </si>
-  <si>
     <t xml:space="preserve">13,68 %</t>
   </si>
   <si>
-    <t xml:space="preserve">-2,77 PP</t>
+    <t xml:space="preserve">10,78 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2,9 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Testkapazität</t>
   </si>
   <si>
-    <t xml:space="preserve">1596994</t>
-  </si>
-  <si>
     <t xml:space="preserve">1785192</t>
   </si>
   <si>
-    <t xml:space="preserve">12 %</t>
+    <t xml:space="preserve">1820400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 %</t>
   </si>
   <si>
     <t xml:space="preserve">Auslastung</t>
   </si>
   <si>
-    <t xml:space="preserve">45 %</t>
-  </si>
-  <si>
     <t xml:space="preserve">60 %</t>
   </si>
   <si>
-    <t xml:space="preserve">15 PP</t>
+    <t xml:space="preserve">58 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2 PP</t>
   </si>
   <si>
     <t xml:space="preserve">R-Wert &amp; 7-Tage-Inzidenz</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reproduktionszahl R</t>
   </si>
   <si>
     <t xml:space="preserve">0,92</t>
   </si>
   <si>
-    <t xml:space="preserve">0,98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  6,5 %</t>
+    <t xml:space="preserve">0,99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  7,6 %</t>
   </si>
   <si>
     <t xml:space="preserve">Neue Fälle je 100.000 EW in 7 Tagen bezogen auf die jeweilige Gruppe:</t>
@@ -120,10 +117,10 @@
     <t xml:space="preserve">174</t>
   </si>
   <si>
-    <t xml:space="preserve">145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-16,7 %</t>
+    <t xml:space="preserve">142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-18,4 %</t>
   </si>
   <si>
     <t xml:space="preserve">Unter-60-Jährige</t>
@@ -132,10 +129,10 @@
     <t xml:space="preserve">169</t>
   </si>
   <si>
-    <t xml:space="preserve">129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-23,7 %</t>
+    <t xml:space="preserve">136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-19,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">Über-60-Jährige</t>
@@ -144,10 +141,10 @@
     <t xml:space="preserve">185</t>
   </si>
   <si>
-    <t xml:space="preserve">157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-15,1 %</t>
+    <t xml:space="preserve">155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-16,2 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon 60-bis-79-Jährige</t>
@@ -156,22 +153,22 @@
     <t xml:space="preserve">138</t>
   </si>
   <si>
-    <t xml:space="preserve">104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-24,6 %</t>
+    <t xml:space="preserve">110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-20,3 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon Über-80-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">336</t>
-  </si>
-  <si>
-    <t xml:space="preserve">283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-15,8 %</t>
+    <t xml:space="preserve">337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10,7 %</t>
   </si>
   <si>
     <t xml:space="preserve">Regionen mit 7-TI bei Über-60-Jährigen:</t>
@@ -183,10 +180,10 @@
     <t xml:space="preserve">395</t>
   </si>
   <si>
-    <t xml:space="preserve">388</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -1,8 %</t>
+    <t xml:space="preserve">389</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -1,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">&gt; 50</t>
@@ -195,10 +192,10 @@
     <t xml:space="preserve">386</t>
   </si>
   <si>
-    <t xml:space="preserve">373</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -3,4 %</t>
+    <t xml:space="preserve">372</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -3,6 %</t>
   </si>
   <si>
     <t xml:space="preserve">Intensivbetten</t>
@@ -250,27 +247,21 @@
     <t xml:space="preserve">Ohne Symptomatik</t>
   </si>
   <si>
-    <t xml:space="preserve">13 %</t>
-  </si>
-  <si>
     <t xml:space="preserve">13,8 %</t>
   </si>
   <si>
+    <t xml:space="preserve"> %</t>
+  </si>
+  <si>
     <t xml:space="preserve"> PP</t>
   </si>
   <si>
     <t xml:space="preserve">Nicht stationär behandelt</t>
   </si>
   <si>
-    <t xml:space="preserve">89,4 %</t>
-  </si>
-  <si>
     <t xml:space="preserve">92,2 %</t>
   </si>
   <si>
-    <t xml:space="preserve">2,8 PP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Intensivmedizinisch behandelt (Schätzung)</t>
   </si>
   <si>
@@ -289,166 +280,169 @@
     <t xml:space="preserve">Neuinfizierte</t>
   </si>
   <si>
-    <t xml:space="preserve">3325</t>
-  </si>
-  <si>
     <t xml:space="preserve">3936</t>
   </si>
   <si>
-    <t xml:space="preserve">18 %</t>
+    <t xml:space="preserve">4210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 %</t>
   </si>
   <si>
     <t xml:space="preserve">Neu stationär behandelt</t>
   </si>
   <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
     <t xml:space="preserve">93</t>
   </si>
   <si>
-    <t xml:space="preserve">19 %</t>
+    <t xml:space="preserve">87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-6 %</t>
   </si>
   <si>
     <t xml:space="preserve">Neu verstorben</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Betreut nach IfSG §36 (u.a. Pflegewohnheim)</t>
   </si>
   <si>
-    <t xml:space="preserve">6055</t>
-  </si>
-  <si>
     <t xml:space="preserve">7389</t>
   </si>
   <si>
-    <t xml:space="preserve">22 %</t>
+    <t xml:space="preserve">8942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 %</t>
   </si>
   <si>
     <t xml:space="preserve">Neuinfizierte über 60 J.</t>
   </si>
   <si>
-    <t xml:space="preserve">5274</t>
-  </si>
-  <si>
     <t xml:space="preserve">6689</t>
   </si>
   <si>
-    <t xml:space="preserve">27 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">870</t>
+    <t xml:space="preserve">8005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 %</t>
   </si>
   <si>
     <t xml:space="preserve">1109</t>
   </si>
   <si>
-    <t xml:space="preserve">1135</t>
+    <t xml:space="preserve">1164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 %</t>
   </si>
   <si>
     <t xml:space="preserve">1477</t>
   </si>
   <si>
-    <t xml:space="preserve">30 %</t>
+    <t xml:space="preserve">1626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 %</t>
   </si>
   <si>
     <t xml:space="preserve">Todesfälle &amp; Sterblichkeit</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 50</t>
+    <t xml:space="preserve">KW 51</t>
   </si>
   <si>
     <t xml:space="preserve">0 bis 59 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">102 ( 0,1%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">112 ( 0,1%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  9,8%</t>
+    <t xml:space="preserve">114 ( 0,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">134 ( 0,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  17,5%</t>
   </si>
   <si>
     <t xml:space="preserve">60 bis 79 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">957 ( 5,0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1168 ( 4,9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 22,0%</t>
+    <t xml:space="preserve">1176 ( 4,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1221 ( 4,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3,8%</t>
   </si>
   <si>
     <t xml:space="preserve">80 Jahre +</t>
   </si>
   <si>
-    <t xml:space="preserve">2740 (19,4%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3447 (18,8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 25,8%</t>
+    <t xml:space="preserve">3476 (18,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3759 (17,8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   8,1%</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">3803 ( 3,0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4728 ( 3,0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 24,3%</t>
+    <t xml:space="preserve">4767 ( 3,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5117 ( 2,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   7,3%</t>
   </si>
   <si>
     <t xml:space="preserve">Übersterblichkeit</t>
   </si>
   <si>
-    <t xml:space="preserve">-49 (-2,9%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">-8 (-0,5%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-83,7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">445 ( 7,0%)</t>
+    <t xml:space="preserve">-123 (-7,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1437,5%</t>
   </si>
   <si>
     <t xml:space="preserve">540 ( 8,4%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 21,3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3141 (29,8%)</t>
+    <t xml:space="preserve">458 ( 7,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -15,2%</t>
   </si>
   <si>
     <t xml:space="preserve">4154 (39,5%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 32,3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3537 (19,0%)</t>
+    <t xml:space="preserve">4234 (39,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1,9%</t>
   </si>
   <si>
     <t xml:space="preserve">4686 (25,2%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 32,5%</t>
+    <t xml:space="preserve">4568 (24,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -2,5%</t>
   </si>
   <si>
     <t xml:space="preserve">Vorwarnzeit</t>
@@ -457,7 +451,7 @@
     <t xml:space="preserve">Bundesdurchschnitt</t>
   </si>
   <si>
-    <t xml:space="preserve">17 Tage</t>
+    <t xml:space="preserve">16 Tage</t>
   </si>
   <si>
     <t xml:space="preserve">kürzeste</t>
@@ -467,18 +461,18 @@
 Thüringen</t>
   </si>
   <si>
-    <t xml:space="preserve">7 Tage
-Brandenburg, Thüringen</t>
+    <t xml:space="preserve">6 Tage
+Brandenburg</t>
   </si>
   <si>
     <t xml:space="preserve">längste</t>
   </si>
   <si>
-    <t xml:space="preserve">45 Tage
+    <t xml:space="preserve">44 Tage
 Bremen</t>
   </si>
   <si>
-    <t xml:space="preserve">39 Tage
+    <t xml:space="preserve">38 Tage
 Bremen</t>
   </si>
   <si>
@@ -509,13 +503,13 @@
     <t xml:space="preserve">Berlin</t>
   </si>
   <si>
-    <t xml:space="preserve">1,07</t>
+    <t xml:space="preserve">1,08</t>
   </si>
   <si>
     <t xml:space="preserve">Brandenburg</t>
   </si>
   <si>
-    <t xml:space="preserve">0,99</t>
+    <t xml:space="preserve">1,01</t>
   </si>
   <si>
     <t xml:space="preserve">Bremen</t>
@@ -524,7 +518,7 @@
     <t xml:space="preserve">Hamburg</t>
   </si>
   <si>
-    <t xml:space="preserve">0,89</t>
+    <t xml:space="preserve">0,90</t>
   </si>
   <si>
     <t xml:space="preserve">Hessen</t>
@@ -542,15 +536,18 @@
     <t xml:space="preserve">Niedersachsen</t>
   </si>
   <si>
+    <t xml:space="preserve">0,98</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nordrhein-Westfalen</t>
   </si>
   <si>
+    <t xml:space="preserve">0,96</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rheinland-Pfalz</t>
   </si>
   <si>
-    <t xml:space="preserve">0,96</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saarland</t>
   </si>
   <si>
@@ -560,18 +557,18 @@
     <t xml:space="preserve">Sachsen</t>
   </si>
   <si>
+    <t xml:space="preserve">0,83</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sachsen-Anhalt</t>
   </si>
   <si>
-    <t xml:space="preserve">1,17</t>
+    <t xml:space="preserve">1,18</t>
   </si>
   <si>
     <t xml:space="preserve">Schleswig-Holstein</t>
   </si>
   <si>
-    <t xml:space="preserve">1,01</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thüringen</t>
   </si>
   <si>
@@ -620,7 +617,7 @@
     <t xml:space="preserve">3,5 %</t>
   </si>
   <si>
-    <t xml:space="preserve">21,1</t>
+    <t xml:space="preserve">22,2</t>
   </si>
   <si>
     <t xml:space="preserve">Belgien</t>
@@ -635,7 +632,7 @@
     <t xml:space="preserve">Vereinigtes Königreich</t>
   </si>
   <si>
-    <t xml:space="preserve">20,2</t>
+    <t xml:space="preserve">21,2</t>
   </si>
   <si>
     <t xml:space="preserve">Niederlande</t>
@@ -653,10 +650,7 @@
     <t xml:space="preserve">Deutschland</t>
   </si>
   <si>
-    <t xml:space="preserve">14,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 %</t>
+    <t xml:space="preserve">14,5</t>
   </si>
   <si>
     <t xml:space="preserve">Rumänien</t>
@@ -665,28 +659,28 @@
     <t xml:space="preserve">2,5 %</t>
   </si>
   <si>
+    <t xml:space="preserve">11,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,8 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frankreich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4 %</t>
+  </si>
+  <si>
     <t xml:space="preserve">Polen</t>
   </si>
   <si>
-    <t xml:space="preserve">10,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,8 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frankreich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,4 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,5 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,9</t>
+    <t xml:space="preserve">11,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,6 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,2</t>
   </si>
   <si>
     <t xml:space="preserve">3,9 %</t>
@@ -695,22 +689,19 @@
     <t xml:space="preserve">2,3 %</t>
   </si>
   <si>
-    <t xml:space="preserve"> 7,6</t>
+    <t xml:space="preserve"> 8,1</t>
   </si>
   <si>
     <t xml:space="preserve">3,8 %</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6,1</t>
+    <t xml:space="preserve"> 6,4</t>
   </si>
   <si>
     <t xml:space="preserve">3,6 %</t>
   </si>
   <si>
     <t xml:space="preserve">1,6 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6,0</t>
   </si>
   <si>
     <t xml:space="preserve">1,4 %</t>
@@ -1154,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1162,21 +1153,21 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -1184,77 +1175,77 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1262,30 +1253,30 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>53</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>57</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>58</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1304,13 +1295,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1318,44 +1309,44 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
         <v>69</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>71</v>
-      </c>
-      <c r="D4" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1365,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1388,49 +1379,49 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>76</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
         <v>78</v>
       </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1438,47 +1429,47 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
         <v>87</v>
-      </c>
-      <c r="B6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
         <v>91</v>
-      </c>
-      <c r="B7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1486,41 +1477,41 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
         <v>102</v>
-      </c>
-      <c r="B11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
         <v>105</v>
@@ -1528,16 +1519,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" t="s">
         <v>108</v>
-      </c>
-      <c r="C13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1556,13 +1547,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1570,63 +1561,63 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
         <v>113</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>114</v>
-      </c>
-      <c r="C2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>118</v>
-      </c>
-      <c r="C3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
         <v>121</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>122</v>
-      </c>
-      <c r="C4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
         <v>125</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>126</v>
-      </c>
-      <c r="C5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
@@ -1634,58 +1625,58 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" t="s">
         <v>130</v>
-      </c>
-      <c r="C7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
         <v>133</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" t="s">
         <v>136</v>
-      </c>
-      <c r="C9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
         <v>139</v>
-      </c>
-      <c r="C10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D10" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1704,13 +1695,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1718,13 +1709,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1732,27 +1723,27 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" t="s">
         <v>145</v>
       </c>
-      <c r="B3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" t="s">
-        <v>147</v>
-      </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
         <v>148</v>
-      </c>
-      <c r="B4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" t="s">
-        <v>150</v>
       </c>
       <c r="D4" t="n">
         <v>-6</v>
@@ -1774,84 +1765,84 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>152</v>
       </c>
-      <c r="C1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" t="s">
-        <v>154</v>
-      </c>
       <c r="E1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="n">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D2" t="n">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C3" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" t="n">
+        <v>145</v>
+      </c>
+      <c r="D4" t="n">
         <v>157</v>
       </c>
-      <c r="B4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4" t="n">
-        <v>152</v>
-      </c>
-      <c r="D4" t="n">
-        <v>164</v>
-      </c>
       <c r="E4" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C5" t="n">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D5" t="n">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E5" t="n">
         <v>21</v>
@@ -1859,50 +1850,50 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C6" t="n">
         <v>240</v>
       </c>
       <c r="D6" t="n">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C7" t="n">
         <v>86</v>
       </c>
       <c r="D7" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" t="n">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D8" t="n">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E8" t="n">
         <v>31</v>
@@ -1910,50 +1901,50 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C9" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" t="n">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E9" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C10" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" t="n">
         <v>153</v>
       </c>
       <c r="E10" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>169</v>
       </c>
       <c r="C11" t="n">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D11" t="n">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E11" t="n">
         <v>21</v>
@@ -1961,19 +1952,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" t="s">
         <v>171</v>
       </c>
-      <c r="B12" t="s">
-        <v>167</v>
-      </c>
       <c r="C12" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E12" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
@@ -1981,24 +1972,24 @@
         <v>172</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C13" t="n">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D13" t="n">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E13" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" t="s">
         <v>174</v>
-      </c>
-      <c r="B14" t="s">
-        <v>175</v>
       </c>
       <c r="C14" t="n">
         <v>109</v>
@@ -2007,24 +1998,24 @@
         <v>113</v>
       </c>
       <c r="E14" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" t="s">
         <v>176</v>
       </c>
-      <c r="B15" t="s">
-        <v>165</v>
-      </c>
       <c r="C15" t="n">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D15" t="n">
         <v>304</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -2035,13 +2026,13 @@
         <v>178</v>
       </c>
       <c r="C16" t="n">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D16" t="n">
         <v>271</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -2049,30 +2040,30 @@
         <v>179</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="C17" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E17" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" t="s">
         <v>181</v>
       </c>
-      <c r="B18" t="s">
-        <v>182</v>
-      </c>
       <c r="C18" t="n">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D18" t="n">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E18" t="n">
         <v>7</v>
@@ -2094,354 +2085,354 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
         <v>183</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>184</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>185</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>186</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>187</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>188</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>189</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>190</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>191</v>
-      </c>
-      <c r="J1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
         <v>193</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="n">
+        <v>889159</v>
+      </c>
+      <c r="D2" t="s">
         <v>194</v>
       </c>
-      <c r="C2" t="n">
-        <v>883906</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>195</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="n">
+        <v>82177</v>
+      </c>
+      <c r="G2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1391</v>
+      </c>
+      <c r="I2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J2" t="s">
         <v>196</v>
-      </c>
-      <c r="F2" t="n">
-        <v>81800</v>
-      </c>
-      <c r="G2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1342</v>
-      </c>
-      <c r="I2" t="s">
-        <v>193</v>
-      </c>
-      <c r="J2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" t="s">
         <v>198</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="n">
+        <v>678839</v>
+      </c>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" t="s">
         <v>199</v>
       </c>
-      <c r="C3" t="n">
-        <v>677209</v>
-      </c>
-      <c r="D3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="n">
+        <v>20435</v>
+      </c>
+      <c r="G3" t="s">
         <v>200</v>
       </c>
-      <c r="F3" t="n">
-        <v>20396</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="n">
+        <v>1100</v>
+      </c>
+      <c r="I3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J3" t="s">
         <v>201</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1043</v>
-      </c>
-      <c r="I3" t="s">
-        <v>201</v>
-      </c>
-      <c r="J3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" t="s">
         <v>203</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="n">
+        <v>925355</v>
+      </c>
+      <c r="D4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
         <v>204</v>
       </c>
-      <c r="C4" t="n">
-        <v>919712</v>
-      </c>
-      <c r="D4" t="s">
-        <v>201</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="n">
+        <v>89429</v>
+      </c>
+      <c r="G4" t="s">
         <v>205</v>
-      </c>
-      <c r="F4" t="n">
-        <v>88747</v>
-      </c>
-      <c r="G4" t="s">
-        <v>206</v>
       </c>
       <c r="H4" t="n">
         <v>693</v>
       </c>
       <c r="I4" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" t="s">
         <v>207</v>
-      </c>
-      <c r="J4" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3405740</v>
+      </c>
+      <c r="D5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" t="s">
         <v>209</v>
       </c>
-      <c r="C5" t="n">
-        <v>3367070</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="n">
+        <v>17221</v>
+      </c>
+      <c r="G5" t="s">
+        <v>202</v>
+      </c>
+      <c r="H5" t="n">
+        <v>542</v>
+      </c>
+      <c r="I5" t="s">
+        <v>194</v>
+      </c>
+      <c r="J5" t="s">
         <v>210</v>
-      </c>
-      <c r="E5" t="s">
-        <v>211</v>
-      </c>
-      <c r="F5" t="n">
-        <v>17164</v>
-      </c>
-      <c r="G5" t="s">
-        <v>203</v>
-      </c>
-      <c r="H5" t="n">
-        <v>509</v>
-      </c>
-      <c r="I5" t="s">
-        <v>212</v>
-      </c>
-      <c r="J5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C6" t="n">
         <v>2252164</v>
       </c>
       <c r="D6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F6" t="n">
+        <v>70422</v>
+      </c>
+      <c r="G6" t="s">
+        <v>212</v>
+      </c>
+      <c r="H6" t="n">
+        <v>393</v>
+      </c>
+      <c r="I6" t="s">
+        <v>214</v>
+      </c>
+      <c r="J6" t="s">
         <v>215</v>
-      </c>
-      <c r="E6" t="s">
-        <v>216</v>
-      </c>
-      <c r="F6" t="n">
-        <v>70093</v>
-      </c>
-      <c r="G6" t="s">
-        <v>195</v>
-      </c>
-      <c r="H6" t="n">
-        <v>352</v>
-      </c>
-      <c r="I6" t="s">
-        <v>195</v>
-      </c>
-      <c r="J6" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C7" t="n">
-        <v>2931686</v>
+        <v>2969091</v>
       </c>
       <c r="D7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F7" t="n">
         <v>53314</v>
       </c>
       <c r="G7" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="H7" t="n">
-        <v>336</v>
+        <v>373</v>
       </c>
       <c r="I7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2381277</v>
+      </c>
+      <c r="D8" t="s">
+        <v>214</v>
+      </c>
+      <c r="E8" t="s">
+        <v>219</v>
+      </c>
+      <c r="F8" t="n">
+        <v>33355</v>
+      </c>
+      <c r="G8" t="s">
+        <v>206</v>
+      </c>
+      <c r="H8" t="n">
+        <v>319</v>
+      </c>
+      <c r="I8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8" t="s">
         <v>220</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2368733</v>
-      </c>
-      <c r="D8" t="s">
-        <v>212</v>
-      </c>
-      <c r="E8" t="s">
-        <v>221</v>
-      </c>
-      <c r="F8" t="n">
-        <v>33213</v>
-      </c>
-      <c r="G8" t="s">
-        <v>207</v>
-      </c>
-      <c r="H8" t="n">
-        <v>305</v>
-      </c>
-      <c r="I8" t="s">
-        <v>215</v>
-      </c>
-      <c r="J8" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C9" t="n">
-        <v>1429612</v>
+        <v>1435582</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F9" t="n">
-        <v>46464</v>
+        <v>46901</v>
       </c>
       <c r="G9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H9" t="n">
-        <v>293</v>
+        <v>309</v>
       </c>
       <c r="I9" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="J9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C10" t="n">
-        <v>691488</v>
+        <v>693644</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F10" t="n">
-        <v>14215</v>
+        <v>14338</v>
       </c>
       <c r="G10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H10" t="n">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="I10" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="J10" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C11" t="n">
-        <v>2038645</v>
+        <v>2050129</v>
       </c>
       <c r="D11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F11" t="n">
-        <v>13066</v>
+        <v>13107</v>
       </c>
       <c r="G11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H11" t="n">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="I11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J11" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>